<commit_message>
Se actualiza documentación de TSP de Gabriel Castillo
</commit_message>
<xml_diff>
--- a/tspi/src/resources/notebook/04. Task and Schedule Plans and Actuals/Planing_Manager/Schedule Planning SCHEDULE_Planing Manager.xlsx
+++ b/tspi/src/resources/notebook/04. Task and Schedule Plans and Actuals/Planing_Manager/Schedule Planning SCHEDULE_Planing Manager.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Downloads\tareas TSP\tareas TSP\por ingeniero y por grupo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Especializacion\PSP\TSP\TSPGit\TSP\tspi\src\resources\notebook\04. Task and Schedule Plans and Actuals\Planing_Manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -307,108 +307,108 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -751,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:G4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -761,222 +761,222 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="3" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11" t="s">
+      <c r="B3" s="37"/>
+      <c r="C3" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="10" t="s">
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="12">
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="42">
         <v>42087</v>
       </c>
-      <c r="L3" s="12"/>
+      <c r="L3" s="42"/>
     </row>
     <row r="4" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="37"/>
+      <c r="C4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="13" t="s">
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="13"/>
+      <c r="L4" s="38"/>
     </row>
     <row r="5" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="10" t="s">
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="13">
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="38">
         <v>1</v>
       </c>
-      <c r="L5" s="13"/>
+      <c r="L5" s="38"/>
     </row>
     <row r="6" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
     </row>
     <row r="7" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="17" t="s">
+      <c r="E7" s="29"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="19"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="30"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="31" t="s">
+      <c r="C8" s="32"/>
+      <c r="D8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="38"/>
-      <c r="I8" s="31" t="s">
+      <c r="H8" s="19"/>
+      <c r="I8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="37" t="s">
+      <c r="J8" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="38"/>
-      <c r="L8" s="31" t="s">
+      <c r="K8" s="19"/>
+      <c r="L8" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="40"/>
-      <c r="L9" s="32"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="16"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="32"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="16"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="32"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="16"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="40"/>
-      <c r="L12" s="32"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="16"/>
     </row>
     <row r="13" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="36"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="33"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="17"/>
     </row>
     <row r="14" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>1</v>
       </c>
-      <c r="B14" s="26">
+      <c r="B14" s="8">
         <v>42091</v>
       </c>
-      <c r="C14" s="27"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="3">
         <v>5</v>
       </c>
@@ -988,21 +988,21 @@
         <f>D14*100/D$27</f>
         <v>7.6923076923076925</v>
       </c>
-      <c r="G14" s="28"/>
-      <c r="H14" s="29"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="11"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="29"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="11"/>
       <c r="L14" s="3"/>
     </row>
     <row r="15" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>2</v>
       </c>
-      <c r="B15" s="26">
+      <c r="B15" s="8">
         <v>42098</v>
       </c>
-      <c r="C15" s="27"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="6">
         <v>5</v>
       </c>
@@ -1014,21 +1014,29 @@
         <f>(D15*100/D$27)+F14</f>
         <v>15.384615384615385</v>
       </c>
-      <c r="G15" s="28"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="5"/>
+      <c r="G15" s="10">
+        <v>4</v>
+      </c>
+      <c r="H15" s="11"/>
+      <c r="I15" s="5">
+        <v>4</v>
+      </c>
+      <c r="J15" s="10">
+        <v>2</v>
+      </c>
+      <c r="K15" s="11"/>
+      <c r="L15" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>3</v>
       </c>
-      <c r="B16" s="26">
+      <c r="B16" s="8">
         <v>42105</v>
       </c>
-      <c r="C16" s="27"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="6">
         <v>5</v>
       </c>
@@ -1040,21 +1048,21 @@
         <f t="shared" ref="F16:F26" si="1">(D16*100/D$27)+F15</f>
         <v>23.076923076923077</v>
       </c>
-      <c r="G16" s="28"/>
-      <c r="H16" s="29"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="29"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="11"/>
       <c r="L16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>4</v>
       </c>
-      <c r="B17" s="26">
+      <c r="B17" s="8">
         <v>42112</v>
       </c>
-      <c r="C17" s="27"/>
+      <c r="C17" s="9"/>
       <c r="D17" s="6">
         <v>5</v>
       </c>
@@ -1066,21 +1074,21 @@
         <f t="shared" si="1"/>
         <v>30.76923076923077</v>
       </c>
-      <c r="G17" s="28"/>
-      <c r="H17" s="29"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="11"/>
       <c r="I17" s="5"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="29"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="11"/>
       <c r="L17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>5</v>
       </c>
-      <c r="B18" s="26">
+      <c r="B18" s="8">
         <v>42119</v>
       </c>
-      <c r="C18" s="27"/>
+      <c r="C18" s="9"/>
       <c r="D18" s="6">
         <v>5</v>
       </c>
@@ -1092,21 +1100,21 @@
         <f t="shared" si="1"/>
         <v>38.46153846153846</v>
       </c>
-      <c r="G18" s="28"/>
-      <c r="H18" s="29"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
       <c r="I18" s="5"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="29"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="11"/>
       <c r="L18" s="5"/>
     </row>
     <row r="19" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>6</v>
       </c>
-      <c r="B19" s="26">
+      <c r="B19" s="8">
         <v>42126</v>
       </c>
-      <c r="C19" s="27"/>
+      <c r="C19" s="9"/>
       <c r="D19" s="6">
         <v>5</v>
       </c>
@@ -1118,21 +1126,21 @@
         <f t="shared" si="1"/>
         <v>46.153846153846153</v>
       </c>
-      <c r="G19" s="28"/>
-      <c r="H19" s="29"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="11"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="29"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="11"/>
       <c r="L19" s="5"/>
     </row>
     <row r="20" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>7</v>
       </c>
-      <c r="B20" s="26">
+      <c r="B20" s="8">
         <v>42133</v>
       </c>
-      <c r="C20" s="27"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="6">
         <v>5</v>
       </c>
@@ -1144,21 +1152,21 @@
         <f t="shared" si="1"/>
         <v>53.846153846153847</v>
       </c>
-      <c r="G20" s="28"/>
-      <c r="H20" s="29"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="11"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="29"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="11"/>
       <c r="L20" s="5"/>
     </row>
     <row r="21" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>8</v>
       </c>
-      <c r="B21" s="26">
+      <c r="B21" s="8">
         <v>42140</v>
       </c>
-      <c r="C21" s="27"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="6">
         <v>5</v>
       </c>
@@ -1170,21 +1178,21 @@
         <f t="shared" si="1"/>
         <v>61.53846153846154</v>
       </c>
-      <c r="G21" s="28"/>
-      <c r="H21" s="29"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="11"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="29"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="11"/>
       <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>9</v>
       </c>
-      <c r="B22" s="26">
+      <c r="B22" s="8">
         <v>42147</v>
       </c>
-      <c r="C22" s="27"/>
+      <c r="C22" s="9"/>
       <c r="D22" s="6">
         <v>5</v>
       </c>
@@ -1196,21 +1204,21 @@
         <f t="shared" si="1"/>
         <v>69.230769230769226</v>
       </c>
-      <c r="G22" s="28"/>
-      <c r="H22" s="29"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="11"/>
       <c r="I22" s="5"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="29"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="11"/>
       <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>10</v>
       </c>
-      <c r="B23" s="26">
+      <c r="B23" s="8">
         <v>42154</v>
       </c>
-      <c r="C23" s="27"/>
+      <c r="C23" s="9"/>
       <c r="D23" s="6">
         <v>5</v>
       </c>
@@ -1222,21 +1230,21 @@
         <f t="shared" si="1"/>
         <v>76.92307692307692</v>
       </c>
-      <c r="G23" s="28"/>
-      <c r="H23" s="29"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="11"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="29"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="11"/>
       <c r="L23" s="5"/>
     </row>
     <row r="24" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>11</v>
       </c>
-      <c r="B24" s="26">
+      <c r="B24" s="8">
         <v>42161</v>
       </c>
-      <c r="C24" s="30"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="6">
         <v>5</v>
       </c>
@@ -1259,10 +1267,10 @@
       <c r="A25" s="4">
         <v>12</v>
       </c>
-      <c r="B25" s="26">
+      <c r="B25" s="8">
         <v>42168</v>
       </c>
-      <c r="C25" s="30"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="6">
         <v>5</v>
       </c>
@@ -1285,10 +1293,10 @@
       <c r="A26" s="4">
         <v>13</v>
       </c>
-      <c r="B26" s="26">
+      <c r="B26" s="8">
         <v>42175</v>
       </c>
-      <c r="C26" s="27"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="6">
         <v>5</v>
       </c>
@@ -1300,11 +1308,11 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G26" s="28"/>
-      <c r="H26" s="29"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="11"/>
       <c r="I26" s="5"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="29"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="11"/>
       <c r="L26" s="5"/>
     </row>
     <row r="27" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1315,6 +1323,51 @@
     </row>
   </sheetData>
   <mergeCells count="61">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="B8:C13"/>
+    <mergeCell ref="L8:L13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="J19:K19"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="G26:H26"/>
     <mergeCell ref="J26:K26"/>
@@ -1331,51 +1384,6 @@
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="B8:C13"/>
-    <mergeCell ref="L8:L13"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:L3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>